<commit_message>
c solved in kW
</commit_message>
<xml_diff>
--- a/Scenarios/c_Multi-Good-MicroGrid/Results/EnergySystemSize.xlsx
+++ b/Scenarios/c_Multi-Good-MicroGrid/Results/EnergySystemSize.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\OneDrive\Documenti\GitHub\MicroGridsPy-MultiEnergy_Paper\Scenarios\c_Multi-Good-MicroGrid\Results\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7F8EF2-DEFA-4DD9-A8BA-0A665580B98D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2265" yWindow="2265" windowWidth="21600" windowHeight="11205" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="510" yWindow="585" windowWidth="17895" windowHeight="8385" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Size" sheetId="1" r:id="rId1"/>
@@ -129,8 +123,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,9 +190,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -488,23 +479,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -527,7 +517,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -547,10 +537,10 @@
         <v>9</v>
       </c>
       <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1729.802117575254</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -570,10 +560,10 @@
         <v>9</v>
       </c>
       <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6553.0566331823038</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -593,10 +583,10 @@
         <v>9</v>
       </c>
       <c r="G4">
-        <v>1387.625459166667</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>98.116476608570437</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -604,19 +594,19 @@
         <v>8</v>
       </c>
       <c r="C5">
-        <v>296.03199999999998</v>
+        <v>297.8</v>
       </c>
       <c r="D5">
-        <v>1157.10682</v>
+        <v>1073.106</v>
       </c>
       <c r="E5">
-        <v>40.387</v>
+        <v>56.100999999999999</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>47.43703977891181</v>
       </c>
       <c r="G5">
-        <v>1493.5258200000001</v>
+        <v>1474.4440397789119</v>
       </c>
     </row>
   </sheetData>
@@ -625,23 +615,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -670,7 +658,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -696,10 +684,10 @@
         <v>9</v>
       </c>
       <c r="I2">
-        <v>0.88502738285761162</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>5.675264476690022</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -725,10 +713,10 @@
         <v>9</v>
       </c>
       <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.34596042351505069</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="2"/>
       <c r="B4" s="1" t="s">
         <v>10</v>
@@ -752,10 +740,10 @@
         <v>9</v>
       </c>
       <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3.6041811482502668</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="2"/>
       <c r="B5" s="1" t="s">
         <v>11</v>
@@ -779,10 +767,10 @@
         <v>9</v>
       </c>
       <c r="I5">
-        <v>0.27752509183333351</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.9623295321714081E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="2"/>
       <c r="B6" s="1" t="s">
         <v>12</v>
@@ -794,22 +782,22 @@
         <v>17</v>
       </c>
       <c r="E6">
-        <v>2.96032E-2</v>
+        <v>2.9780000000000001E-2</v>
       </c>
       <c r="F6">
-        <v>0.115710682</v>
+        <v>0.10731060000000001</v>
       </c>
       <c r="G6">
-        <v>4.0387000000000001E-3</v>
+        <v>5.6101000000000007E-3</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>4.7437039778911814E-3</v>
       </c>
       <c r="I6">
-        <v>0.14935258200000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.14744440397789119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -835,10 +823,10 @@
         <v>9</v>
       </c>
       <c r="I7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>9.6582498539022024E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="2"/>
       <c r="B8" s="1" t="s">
         <v>10</v>
@@ -862,10 +850,10 @@
         <v>9</v>
       </c>
       <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.006186826078123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="2"/>
       <c r="B9" s="1" t="s">
         <v>11</v>
@@ -889,10 +877,10 @@
         <v>9</v>
       </c>
       <c r="I9">
-        <v>0.3873863158132132</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2.7391382986583088E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="2"/>
       <c r="B10" s="1" t="s">
         <v>12</v>
@@ -904,22 +892,22 @@
         <v>17</v>
       </c>
       <c r="E10">
-        <v>6.1982906708677159E-3</v>
+        <v>6.2353088915536358E-3</v>
       </c>
       <c r="F10">
-        <v>2.4227395712637181E-2</v>
+        <v>2.2468594302819191E-2</v>
       </c>
       <c r="G10">
-        <v>8.4561927536325274E-4</v>
+        <v>1.1746375558262269E-3</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>9.9323235702630059E-4</v>
       </c>
       <c r="I10">
-        <v>3.1271305658868147E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3.0871773107225359E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -945,10 +933,10 @@
         <v>9</v>
       </c>
       <c r="I11">
-        <v>3.9492087552196763E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.39702272491414548</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -977,7 +965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -1016,19 +1004,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="C1" s="1" t="s">
         <v>24</v>
       </c>
@@ -1039,7 +1027,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
@@ -1047,16 +1035,16 @@
         <v>27</v>
       </c>
       <c r="C2">
-        <v>1670.3766851</v>
+        <v>296111.13119142258</v>
       </c>
       <c r="D2">
-        <v>371.84483853</v>
+        <v>145482.79193819009</v>
       </c>
       <c r="E2">
-        <v>2042.2215236300001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>441593.92312961258</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -1070,10 +1058,10 @@
         <v>9</v>
       </c>
       <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.36747665930473272</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
@@ -1087,10 +1075,10 @@
         <v>9</v>
       </c>
       <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.63252334069526728</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -1098,16 +1086,16 @@
         <v>29</v>
       </c>
       <c r="C5">
-        <v>7.7388632248696118E-2</v>
+        <v>0.16133879840240151</v>
       </c>
       <c r="D5">
-        <v>1.0101010101010099</v>
+        <v>1.010097467358436</v>
       </c>
       <c r="E5">
-        <v>0.24721559740620461</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.44096171523593591</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
@@ -1121,7 +1109,7 @@
         <v>9</v>
       </c>
       <c r="E6">
-        <v>7.5350687817872649E-3</v>
+        <v>1.2527700483863421E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>